<commit_message>
Updated Hydrants to use new PM Shift Codes and added UserStatsu1.
Note that other equipment stored procedures needed to be updated to
include a null value for UserStatus1 because this change added it as a
new field for the entire Equipment load.
</commit_message>
<xml_diff>
--- a/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
+++ b/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbuck\Documents\Projects\NNWW\AssetWorks Conversion\Loading\Equipment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\REPOS\AssetWorksConversion\Loading\Equipment\CurrentCycle\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5784"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="ValidatedSource" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>EquipmentID</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>StationLocation</t>
+  </si>
+  <si>
+    <t>UserStatus1</t>
   </si>
 </sst>
 </file>
@@ -531,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -655,69 +658,72 @@
         <v>35</v>
       </c>
       <c r="AM1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -734,14 +740,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Changes to Equipment Loading SSIS package related to IndividualPm
Fixed bug which caused IndividualPM tab to not be produced in load file.
Per BA also added grouprow identifier to primary tab.  CreateTable sql
updated to reflect modified table.  Fixed formatting of
TargetEquipmentIndividualPM table.
</commit_message>
<xml_diff>
--- a/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
+++ b/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5796" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidatedSource" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>EquipmentID</t>
   </si>
@@ -208,6 +208,39 @@
   </si>
   <si>
     <t>UserStatus1</t>
+  </si>
+  <si>
+    <t>2424</t>
+  </si>
+  <si>
+    <t>[KEY]</t>
+  </si>
+  <si>
+    <t>12359:3</t>
+  </si>
+  <si>
+    <t>12359:6</t>
+  </si>
+  <si>
+    <t>12359:17</t>
+  </si>
+  <si>
+    <t>12359:18</t>
+  </si>
+  <si>
+    <t>PMKey</t>
+  </si>
+  <si>
+    <t>PMServiceType</t>
+  </si>
+  <si>
+    <t>NextDueDate</t>
+  </si>
+  <si>
+    <t>NumberOfTimeUnits</t>
+  </si>
+  <si>
+    <t>TimeUnit</t>
   </si>
 </sst>
 </file>
@@ -249,11 +282,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,13 +574,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView topLeftCell="AD1" workbookViewId="0">
       <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -734,31 +772,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
+      <c r="B1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor formatting change to template
</commit_message>
<xml_diff>
--- a/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
+++ b/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5796" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5796"/>
   </bookViews>
   <sheets>
     <sheet name="ValidatedSource" sheetId="1" r:id="rId1"/>
@@ -574,11 +574,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI1"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -774,15 +836,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated template per BA (removed unused columns)
</commit_message>
<xml_diff>
--- a/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
+++ b/Loading/Equipment/CurrentCycle/Data/Equipment - Template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>EquipmentID</t>
   </si>
@@ -187,18 +187,6 @@
   </si>
   <si>
     <t>NextPMDueDate</t>
-  </si>
-  <si>
-    <t>IndividualPMService</t>
-  </si>
-  <si>
-    <t>IndividualPMDateNextDue</t>
-  </si>
-  <si>
-    <t>IndividualPMNumberofTimeUnits</t>
-  </si>
-  <si>
-    <t>IndividualPMTimeUnit</t>
   </si>
   <si>
     <t>Control</t>
@@ -572,11 +560,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -636,15 +622,11 @@
     <col min="55" max="55" width="9" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -716,7 +698,7 @@
         <v>22</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>23</v>
@@ -758,7 +740,7 @@
         <v>35</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AN1" s="2" t="s">
         <v>36</v>
@@ -813,18 +795,6 @@
       </c>
       <c r="BE1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="BF1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -836,9 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -852,42 +820,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>